<commit_message>
import data & add instansi
</commit_message>
<xml_diff>
--- a/assets/file/Alumni.xlsx
+++ b/assets/file/Alumni.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\siluni-ts\assets\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B4771B93-7DE0-45D8-A60C-34010371F76B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB23A62E-5EE4-44AD-9C6F-6872AAF45248}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="15375" windowHeight="7875" xr2:uid="{91B26D3F-09CD-463D-8530-4F7A088E41A1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{91B26D3F-09CD-463D-8530-4F7A088E41A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>NIM</t>
   </si>
@@ -38,13 +38,16 @@
     <t>Nama</t>
   </si>
   <si>
-    <t>Jenis Kelamin</t>
-  </si>
-  <si>
     <t>Tahun Masuk</t>
   </si>
   <si>
-    <t>Tanggal Lulus</t>
+    <t>Jenis Kelamin (Laki-laki/Perempuan)</t>
+  </si>
+  <si>
+    <t>Tanggal Lulus (dd/M)</t>
+  </si>
+  <si>
+    <t>Tahun Lulus</t>
   </si>
 </sst>
 </file>
@@ -60,15 +63,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -76,12 +85,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,34 +421,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FE21F96-7C77-43DE-A6D5-EEE6CC0378D4}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" customWidth="1"/>
+    <col min="3" max="3" width="33.42578125" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>